<commit_message>
update big gird system
</commit_message>
<xml_diff>
--- a/map.xlsx
+++ b/map.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\73133\Desktop\AGV-v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\73133\Desktop\ST-Astar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D17CE3-0DFF-4DA2-B07A-B77E818BAB13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF7FE85-6F05-4A27-A740-C191CC3DC9EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{882A7C78-D428-1446-AB7B-197BB25BD2CE}"/>
+    <workbookView xWindow="1800" yWindow="1095" windowWidth="21600" windowHeight="11295" xr2:uid="{882A7C78-D428-1446-AB7B-197BB25BD2CE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -386,12 +386,15 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="8" width="3.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2</v>
       </c>
@@ -417,7 +420,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -443,7 +446,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -469,7 +472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -495,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -521,7 +524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -547,7 +550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -573,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -599,7 +602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
@@ -625,7 +628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>

</xml_diff>